<commit_message>
Query and table name updated
</commit_message>
<xml_diff>
--- a/excel-readWrite/src/main/resources/Students.xlsx
+++ b/excel-readWrite/src/main/resources/Students.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RAHUL DAS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PublicGit\ExcelFileReadWrite\excel-readWrite\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19365" windowHeight="9390"/>
   </bookViews>
   <sheets>
-    <sheet name="Students" sheetId="1" r:id="rId1"/>
+    <sheet name="STUDENTS" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,12 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
@@ -75,12 +69,18 @@
   </si>
   <si>
     <t>K</t>
+  </si>
+  <si>
+    <t>First_Name</t>
+  </si>
+  <si>
+    <t>Last_Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -133,8 +133,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F6" totalsRowShown="0">
   <autoFilter ref="A1:F6"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="First Name"/>
-    <tableColumn id="2" name="Last Name"/>
+    <tableColumn id="1" name="First_Name"/>
+    <tableColumn id="2" name="Last_Name"/>
     <tableColumn id="3" name="Age"/>
     <tableColumn id="4" name="Gender"/>
     <tableColumn id="5" name="Height"/>
@@ -410,51 +410,51 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
       <c r="C2">
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E2">
         <v>175</v>
@@ -463,18 +463,18 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <v>163</v>
@@ -483,18 +483,18 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E4">
         <v>189</v>
@@ -503,15 +503,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E5">
         <v>175</v>
@@ -520,18 +520,18 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E6">
         <v>170</v>

</xml_diff>